<commit_message>
them tinh nang quan ly danh muc
</commit_message>
<xml_diff>
--- a/ProjectLaravel/tailieu.xlsx
+++ b/ProjectLaravel/tailieu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bai-tap\ProjectLaravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2602FD8-0B1B-43BB-B3DC-1845F62914C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FC7C1E-8814-4651-B481-4CFEBCAD77FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{7AAE7466-426B-4D75-981B-E0A1C33A8874}"/>
   </bookViews>
@@ -1524,7 +1524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1534,7 +1534,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2832,6 +2831,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>176168</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>373407</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>37137</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A0F0D28-FDFA-3F14-6C36-1135BC97B80B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="967740" y="16635368"/>
+          <a:ext cx="11864367" cy="6078889"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3490,8 +3538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E672DE6-EBF4-4E50-8053-28064B37CF8D}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P82" sqref="P82"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="P90" sqref="P90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3532,7 +3580,6 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -4533,5 +4580,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>